<commit_message>
Solve SetInputSpace - dimension problem
</commit_message>
<xml_diff>
--- a/ArtigoKrigingVsg/benchmark/KrigingMetrics.xlsx
+++ b/ArtigoKrigingVsg/benchmark/KrigingMetrics.xlsx
@@ -522,52 +522,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.6675858078539003</v>
+        <v>0.6675858082427026</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1973354240033358</v>
+        <v>0.1973354237725259</v>
       </c>
       <c r="C2" t="n">
-        <v>0.278102441442457</v>
+        <v>0.2781024412082834</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4442245198132762</v>
+        <v>0.4442245195534865</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2.950656151618782e-28</v>
+        <v>6.979693377975784e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>9.233000623380752e-15</v>
+        <v>4.406330720924272e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>1.717747406232587e-14</v>
+        <v>8.354455923622905e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6513796842871884</v>
+        <v>0.6513796849758856</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2442157713035413</v>
+        <v>0.2442157708210946</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4838358801666359</v>
+        <v>0.4838358795907293</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4941819212633555</v>
+        <v>0.4941819207752289</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6430580180165908</v>
+        <v>0.7443853761732526</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2062651184997909</v>
+        <v>0.1251941513667706</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2832334326511898</v>
+        <v>0.1597491092106763</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4541641977300621</v>
+        <v>0.3538278555551705</v>
       </c>
     </row>
   </sheetData>
@@ -673,52 +673,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.708270789581652</v>
+        <v>0.7082707905677209</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1731830613500433</v>
+        <v>0.1731830607646702</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2437041929119865</v>
+        <v>0.2437041923490998</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4161526899469031</v>
+        <v>0.4161526892435878</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>4.260468652244135e-24</v>
+        <v>7.036755824661521e-24</v>
       </c>
       <c r="G2" t="n">
-        <v>8.88231622782968e-13</v>
+        <v>1.431912009762658e-12</v>
       </c>
       <c r="H2" t="n">
-        <v>2.064090272309846e-12</v>
+        <v>2.652688414545048e-12</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6686518884711664</v>
+        <v>0.6686518898700511</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2321162335635282</v>
+        <v>0.2321162325835804</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4502923182597695</v>
+        <v>0.4502923171128647</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4817844264435373</v>
+        <v>0.481784425426539</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6788904194797192</v>
+        <v>0.7946388445521382</v>
       </c>
       <c r="N2" t="n">
-        <v>0.185558743494937</v>
+        <v>0.1005811607923515</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2536856068955126</v>
+        <v>0.1272597757958034</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4307652997804454</v>
+        <v>0.3171453307118859</v>
       </c>
     </row>
   </sheetData>
@@ -824,52 +824,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.6292361932295476</v>
+        <v>0.6292361889479723</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2201014118614447</v>
+        <v>0.2201014144031727</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3093648929298694</v>
+        <v>0.3093648956339847</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4691496689345999</v>
+        <v>0.4691496716434667</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1.31579533800536e-29</v>
+        <v>1.233457981022916e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>1.739367296444301e-15</v>
+        <v>1.525742510176214e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>3.627389333949913e-15</v>
+        <v>3.512062045327384e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5831568703044034</v>
+        <v>0.5831568642345634</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2920072693498829</v>
+        <v>0.292007273601932</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5586679318562336</v>
+        <v>0.5586679374723076</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5403769696701395</v>
+        <v>0.5403769736044755</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6173602289541866</v>
+        <v>0.7132259063696762</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2211150318573791</v>
+        <v>0.1404553415158181</v>
       </c>
       <c r="O2" t="n">
-        <v>0.3039592536959999</v>
+        <v>0.1803210790901188</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4702287016520568</v>
+        <v>0.3747737204178251</v>
       </c>
     </row>
   </sheetData>
@@ -975,52 +975,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-0.05017696330948063</v>
+        <v>-0.05017696330948196</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6234304107031897</v>
+        <v>0.6234304107031905</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5921680198200971</v>
+        <v>0.5921680198200978</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7895760955748279</v>
+        <v>0.7895760955748283</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2.533393927912895e-30</v>
+        <v>2.194841122755544e-30</v>
       </c>
       <c r="G2" t="n">
-        <v>7.790200092990539e-16</v>
+        <v>6.987666884789323e-16</v>
       </c>
       <c r="H2" t="n">
-        <v>1.591663886601972e-15</v>
+        <v>1.481499619559703e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.08863502004839741</v>
+        <v>-0.08863502004839785</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7626114403159988</v>
+        <v>0.7626114403159991</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9501502032838554</v>
+        <v>0.9501502032838559</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8732762680366385</v>
+        <v>0.8732762680366386</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.1774605127901776</v>
+        <v>-0.01636870287358216</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6804159904361691</v>
+        <v>0.4977939654902045</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6427217967843691</v>
+        <v>0.3979895811419075</v>
       </c>
       <c r="P2" t="n">
-        <v>0.824873317810783</v>
+        <v>0.7055451548201607</v>
       </c>
     </row>
   </sheetData>
@@ -1126,52 +1126,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.3200064936047624</v>
+        <v>0.3200064928743519</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4036735195861995</v>
+        <v>0.4036735200198026</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4646543708451828</v>
+        <v>0.4646543711342551</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6353530668740015</v>
+        <v>0.6353530672152317</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>2.309472473045473e-30</v>
+        <v>2.576123893612367e-30</v>
       </c>
       <c r="G2" t="n">
-        <v>6.135415262294454e-16</v>
+        <v>7.892850043672255e-16</v>
       </c>
       <c r="H2" t="n">
-        <v>1.519694861821107e-15</v>
+        <v>1.605030807683257e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.284070207174553</v>
+        <v>0.2840702064200564</v>
       </c>
       <c r="J2" t="n">
-        <v>0.5015236883041631</v>
+        <v>0.5015236888327036</v>
       </c>
       <c r="K2" t="n">
-        <v>0.770008918130583</v>
+        <v>0.770008918542557</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7081833719483698</v>
+        <v>0.7081833723215363</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2701359277555211</v>
+        <v>0.3801382620230105</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4217646198794425</v>
+        <v>0.3035939927418204</v>
       </c>
       <c r="O2" t="n">
-        <v>0.492472846031031</v>
+        <v>0.3031425412414653</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6494340766232108</v>
+        <v>0.5509936412898251</v>
       </c>
     </row>
   </sheetData>
@@ -1277,52 +1277,52 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.6416256096658581</v>
+        <v>0.6416256090604304</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2127465190699279</v>
+        <v>0.2127465194293359</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3042790979994127</v>
+        <v>0.3042790984108429</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4612445328347295</v>
+        <v>0.4612445332243363</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>1.067632844904583e-29</v>
+        <v>2.74346923043347e-29</v>
       </c>
       <c r="G2" t="n">
-        <v>1.744510984666794e-15</v>
+        <v>2.418830424768703e-15</v>
       </c>
       <c r="H2" t="n">
-        <v>3.267465141213572e-15</v>
+        <v>5.237813695076859e-15</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5855851095401134</v>
+        <v>0.5855851084770898</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2903062373355957</v>
+        <v>0.2903062380802658</v>
       </c>
       <c r="K2" t="n">
-        <v>0.5498088027053577</v>
+        <v>0.5498088035944768</v>
       </c>
       <c r="L2" t="n">
-        <v>0.5388007399174538</v>
+        <v>0.5388007406084978</v>
       </c>
       <c r="M2" t="n">
-        <v>0.627796279979203</v>
+        <v>0.7270330263336232</v>
       </c>
       <c r="N2" t="n">
-        <v>0.2150843786700359</v>
+        <v>0.1336929323827744</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2990381110363547</v>
+        <v>0.1757018704271285</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4637719037091789</v>
+        <v>0.3656404413939662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>